<commit_message>
new descriptive stats added
</commit_message>
<xml_diff>
--- a/data/results.xlsx
+++ b/data/results.xlsx
@@ -423,13 +423,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.25</v>
+        <v>0.6667</v>
       </c>
       <c r="C2">
-        <v>0.475</v>
+        <v>0.7375</v>
       </c>
       <c r="D2">
-        <v>0.5385</v>
+        <v>0.7692</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -443,13 +443,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.7272999999999999</v>
+        <v>0.75</v>
       </c>
       <c r="C3">
-        <v>0.775</v>
+        <v>0.8</v>
       </c>
       <c r="D3">
-        <v>0.7692</v>
+        <v>0.8462</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -463,13 +463,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.4</v>
+        <v>0.6667</v>
       </c>
       <c r="C4">
-        <v>0.5125</v>
+        <v>0.7375</v>
       </c>
       <c r="D4">
-        <v>0.5385</v>
+        <v>0.7692</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -503,13 +503,13 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.6667</v>
+        <v>0.2857</v>
       </c>
       <c r="C6">
-        <v>0.75</v>
+        <v>0.5833</v>
       </c>
       <c r="D6">
-        <v>0.7692</v>
+        <v>0.6153999999999999</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -523,10 +523,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="C7">
-        <v>0.5119</v>
+        <v>0.5238</v>
       </c>
       <c r="D7">
         <v>0.5385</v>
@@ -543,13 +543,13 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.3333</v>
+        <v>0.5714</v>
       </c>
       <c r="C8">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="D8">
-        <v>0.6667</v>
+        <v>0.75</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
@@ -583,13 +583,13 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.2857</v>
+        <v>0.5714</v>
       </c>
       <c r="C10">
-        <v>0.5286</v>
+        <v>0.7</v>
       </c>
       <c r="D10">
-        <v>0.5833</v>
+        <v>0.75</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -603,13 +603,13 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.5714</v>
+        <v>0.8889</v>
       </c>
       <c r="C11">
-        <v>0.6786</v>
+        <v>0.9286</v>
       </c>
       <c r="D11">
-        <v>0.7272999999999999</v>
+        <v>0.9091</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
@@ -623,13 +623,13 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0.8889</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0.9286</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0.9091</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -643,13 +643,13 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="C13">
-        <v>0.625</v>
+        <v>0.8571</v>
       </c>
       <c r="D13">
-        <v>0.7272999999999999</v>
+        <v>0.8182</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
@@ -663,13 +663,13 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.6667</v>
+        <v>0.6</v>
       </c>
       <c r="C14">
-        <v>0.7167</v>
+        <v>0.6333</v>
       </c>
       <c r="D14">
-        <v>0.7272999999999999</v>
+        <v>0.6364</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
@@ -683,13 +683,13 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.6667</v>
+        <v>0.5</v>
       </c>
       <c r="C15">
-        <v>0.7167</v>
+        <v>0.6167</v>
       </c>
       <c r="D15">
-        <v>0.7272999999999999</v>
+        <v>0.6364</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
@@ -703,13 +703,13 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.6667</v>
+        <v>0.4444</v>
       </c>
       <c r="C16">
-        <v>0.7167</v>
+        <v>0.5333</v>
       </c>
       <c r="D16">
-        <v>0.7272999999999999</v>
+        <v>0.5455</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>

</xml_diff>